<commit_message>
include ragwitz and van den berg
</commit_message>
<xml_diff>
--- a/output/barplot_values_data.xlsx
+++ b/output/barplot_values_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -574,7 +574,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -625,7 +625,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -676,7 +676,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -727,7 +727,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -778,7 +778,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -829,7 +829,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -931,7 +931,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>pkm/cap/year</t>
+          <t>passenger-km/cap/year</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>m2/cap</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>m2/capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1307,7 +1307,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>m2/cap</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>m2/cap</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>m2</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -2349,23 +2349,23 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Rao and Min (2018)</t>
+          <t>van den Berg et al. (2021)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>WD-DLS</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>decent living standard</t>
+          <t>Behavioural change</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>per capita living space, minimum/basic need with 2 people / flat</t>
+          <t>floor space per capita rural/urban average</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2379,10 +2379,16 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>15</v>
-      </c>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+        <v>43.3</v>
+      </c>
+      <c r="I40" t="n">
+        <v>22.78</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Grubler et al. (2018)</t>
+        </is>
+      </c>
       <c r="K40" t="b">
         <v>1</v>
       </c>
@@ -2406,7 +2412,7 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>per capita living space, minimum/basic need with 3 or more people / flat</t>
+          <t>per capita living space, minimum/basic need with 2 people / flat</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2420,7 +2426,7 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
@@ -2431,68 +2437,58 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>UBA (2021)</t>
+          <t>Rao and Min (2018)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>WD-DLS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>GreenSupreme</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Industry</t>
-        </is>
-      </c>
+          <t>decent living standard</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Steel production</t>
+          <t>per capita living space, minimum/basic need with 3 or more people / flat</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>steel production per capita and year</t>
+          <t>living space per capita</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>négaWatt et al. (2023)</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
       <c r="K42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ADEME (2022)</t>
+          <t>UBA (2021)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>S1: Low production</t>
+          <t>GreenSupreme</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2502,7 +2498,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>steel production per capita</t>
+          <t>Steel production</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2512,14 +2508,14 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>0.08</v>
+        <v>0.44</v>
       </c>
       <c r="I43" t="n">
-        <v>0.22</v>
+        <v>0.48</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -2533,7 +2529,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>négaWatt (2022)</t>
+          <t>ADEME (2022)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2543,7 +2539,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>S1: Low production</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2553,7 +2549,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>steel production</t>
+          <t>steel production per capita</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2563,11 +2559,11 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="I44" t="n">
         <v>0.22</v>
@@ -2584,7 +2580,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>RTE (2021)</t>
+          <t>négaWatt (2022)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2594,7 +2590,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Sufficiency</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2604,7 +2600,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Steel production</t>
+          <t>steel production</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2614,11 +2610,11 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="I45" t="n">
         <v>0.22</v>
@@ -2635,17 +2631,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Barrett et al. (2022)</t>
+          <t>RTE (2021)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Transform</t>
+          <t>Sufficiency</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2655,7 +2651,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>per capita iron and steel production</t>
+          <t>Steel production</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2665,14 +2661,14 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
       <c r="I46" t="n">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -2686,17 +2682,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Climact (2024)</t>
+          <t>Barrett et al. (2022)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Net Zero 2040</t>
+          <t>Transform</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2706,7 +2702,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>steel production</t>
+          <t>per capita iron and steel production</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2716,14 +2712,14 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>0.29</v>
+        <v>0.06</v>
       </c>
       <c r="I47" t="n">
-        <v>0.34</v>
+        <v>0.11</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -2737,7 +2733,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>Climact (2024)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2747,7 +2743,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>EU path</t>
+          <t>Net Zero 2040</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2757,7 +2753,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Production of crude steel per capita</t>
+          <t>steel production</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2767,11 +2763,11 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="I48" t="n">
         <v>0.34</v>
@@ -2788,17 +2784,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Climact (2018)</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>EU28</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>demand</t>
+          <t>EU path</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2808,7 +2804,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>steel production</t>
+          <t>Production of crude steel per capita</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2818,14 +2814,14 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="I49" t="n">
-        <v>0.27</v>
+        <v>0.34</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -2839,17 +2835,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>Climact (2018)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>EU28+CH</t>
+          <t>EU28</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Life / Lever 4</t>
+          <t>demand</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2869,18 +2865,18 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>0.31</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I50" t="n">
-        <v>0.32</v>
+        <v>0.27</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K50" t="b">
@@ -2890,23 +2886,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Grubler et al. (2018)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>EU28+CH</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
+          <t>Life / Lever 4</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>steel demand</t>
+          <t>steel production</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2916,28 +2916,28 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H51" t="n">
-        <v>0.06</v>
+        <v>0.31</v>
       </c>
       <c r="I51" t="n">
-        <v>0.24</v>
+        <v>0.32</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="K51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Grubler et al. (2018)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2947,13 +2947,13 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>NZE</t>
+          <t>LED</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Steel production</t>
+          <t>steel demand</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2967,7 +2967,7 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>0.21</v>
+        <v>0.06</v>
       </c>
       <c r="I52" t="n">
         <v>0.24</v>
@@ -2984,32 +2984,28 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>UBA (2021)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>GreenSupreme</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Industry</t>
-        </is>
-      </c>
+          <t>NZE</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Cement production per capita and year</t>
+          <t>Steel production</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>cement production per capita and year</t>
+          <t>steel production per capita and year</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -3018,34 +3014,34 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="I53" t="n">
-        <v>0.41</v>
+        <v>0.24</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="K53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ADEME (2022)</t>
+          <t>UBA (2021)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>S1: Low production</t>
+          <t>GreenSupreme</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3055,7 +3051,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>cement production</t>
+          <t>Cement production per capita and year</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3065,14 +3061,14 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>0.06</v>
+        <v>0.22</v>
       </c>
       <c r="I54" t="n">
-        <v>0.26</v>
+        <v>0.41</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -3086,7 +3082,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>RTE (2021)</t>
+          <t>ADEME (2022)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3096,7 +3092,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Sufficiency</t>
+          <t>S1: Low production</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -3106,7 +3102,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Cement production</t>
+          <t>cement production</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3116,11 +3112,11 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H55" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="I55" t="n">
         <v>0.26</v>
@@ -3137,17 +3133,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Gaur et al. (2022)</t>
+          <t>RTE (2021)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ILED</t>
+          <t>Sufficiency</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -3167,14 +3163,14 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>0.33</v>
+        <v>0.12</v>
       </c>
       <c r="I56" t="n">
-        <v>0.66</v>
+        <v>0.26</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -3188,17 +3184,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Barrett et al. (2022)</t>
+          <t>Gaur et al. (2022)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Transform</t>
+          <t>ILED</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -3208,7 +3204,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>per capita cement production</t>
+          <t>Cement production</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3218,14 +3214,14 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>0.08</v>
+        <v>0.33</v>
       </c>
       <c r="I57" t="n">
-        <v>0.14</v>
+        <v>0.66</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -3239,17 +3235,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Climact (2024)</t>
+          <t>Barrett et al. (2022)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Net Zero 2040</t>
+          <t>Transform</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3259,7 +3255,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>cement production</t>
+          <t>per capita cement production</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3269,14 +3265,14 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H58" t="n">
-        <v>0.18</v>
+        <v>0.08</v>
       </c>
       <c r="I58" t="n">
-        <v>0.37</v>
+        <v>0.14</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -3290,7 +3286,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>Climact (2024)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -3300,7 +3296,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>EU path</t>
+          <t>Net Zero 2040</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3310,7 +3306,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Production of cement per capita</t>
+          <t>cement production</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3320,11 +3316,11 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H59" t="n">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
       <c r="I59" t="n">
         <v>0.37</v>
@@ -3341,17 +3337,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Climact (2018)</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>EU28</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>demand</t>
+          <t>EU path</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3361,7 +3357,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>cement production</t>
+          <t>Production of cement per capita</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -3371,14 +3367,14 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="I60" t="n">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -3392,17 +3388,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>Climact (2018)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>EU28+CH</t>
+          <t>EU28</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Life / Lever 4</t>
+          <t>demand</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -3422,18 +3418,18 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>0.19</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I61" t="n">
         <v>0.34</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K61" t="b">
@@ -3443,23 +3439,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Grubler et al. (2018)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>EU28+CH</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
+          <t>Life / Lever 4</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>cement demand</t>
+          <t>cement production</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3469,28 +3469,28 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>t/cap/year</t>
+          <t>ton/cap/year</t>
         </is>
       </c>
       <c r="H62" t="n">
-        <v>0.44</v>
+        <v>0.19</v>
       </c>
       <c r="I62" t="n">
-        <v>0.55</v>
+        <v>0.34</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="K62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Grubler et al. (2018)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -3500,13 +3500,13 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>NZE</t>
+          <t>LED</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Cement production</t>
+          <t>cement demand</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3520,7 +3520,7 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="I63" t="n">
         <v>0.55</v>
@@ -3537,68 +3537,64 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>UBA (2021)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>GreenSupreme</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Industry</t>
-        </is>
-      </c>
+          <t>NZE</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Final energy demand per capita industry</t>
+          <t>Cement production</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>final energy demand per capita and year | industry</t>
+          <t>cement production per capita and year</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>GJ/cap/year</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="H64" t="n">
-        <v>18.78</v>
+        <v>0.42</v>
       </c>
       <c r="I64" t="n">
-        <v>31.36</v>
+        <v>0.55</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>UBA (2021)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="K64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>RTE (2021)</t>
+          <t>UBA (2021)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Sufficiency</t>
+          <t>GreenSupreme</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -3608,7 +3604,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Final energy demand | Industry</t>
+          <t>Final energy demand per capita industry</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3622,14 +3618,14 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>13.68</v>
+        <v>18.78</v>
       </c>
       <c r="I65" t="n">
-        <v>19.99</v>
+        <v>31.36</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>UBA (2021)</t>
         </is>
       </c>
       <c r="K65" t="b">
@@ -3639,17 +3635,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ADEME (2022)</t>
+          <t>Ragwitz et al. (2023)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>S1: Low production</t>
+          <t>Nachfrage+Tech</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -3659,7 +3655,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Final energy demand per capita and year | Industry</t>
+          <t>Final Energy Demand | Industry</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3673,10 +3669,10 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>14.46</v>
+        <v>24.47</v>
       </c>
       <c r="I66" t="n">
-        <v>19.99</v>
+        <v>29.12</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -3690,7 +3686,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>négaWatt (2022)</t>
+          <t>RTE (2021)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3700,7 +3696,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>Sufficiency</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3710,7 +3706,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>final energy consumption | Industry (including non-national)</t>
+          <t>Final energy demand | Industry</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3724,7 +3720,7 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>17.72</v>
+        <v>13.68</v>
       </c>
       <c r="I67" t="n">
         <v>19.99</v>
@@ -3741,17 +3737,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Gaur et al. (2022)</t>
+          <t>ADEME (2022)</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ILED</t>
+          <t>S1: Low production</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3761,7 +3757,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Final energy demand per capita | Industry</t>
+          <t>Final energy demand per capita and year | Industry</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3775,10 +3771,10 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>11.16</v>
+        <v>14.46</v>
       </c>
       <c r="I68" t="n">
-        <v>19.58</v>
+        <v>19.99</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -3792,17 +3788,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Barrett et al. (2022)</t>
+          <t>négaWatt (2022)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Transform</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3812,7 +3808,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>final energy demand per capita | Industry</t>
+          <t>final energy consumption | Industry (including non-national)</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3822,14 +3818,14 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>GJ/person/year</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="H69" t="n">
-        <v>13.1</v>
+        <v>17.72</v>
       </c>
       <c r="I69" t="n">
-        <v>13.09</v>
+        <v>19.99</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -3843,17 +3839,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Climact (2024)</t>
+          <t>Gaur et al. (2022)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Net Zero 2040</t>
+          <t>ILED</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3863,7 +3859,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>final energy demand industry</t>
+          <t>Final energy demand per capita | Industry</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3877,10 +3873,10 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>14.78</v>
+        <v>11.16</v>
       </c>
       <c r="I70" t="n">
-        <v>24.2</v>
+        <v>19.58</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -3894,17 +3890,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>Barrett et al. (2022)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>EU path</t>
+          <t>Transform</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3914,7 +3910,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>per capita Total FEC of industry (excl. consumption of the energy sector)</t>
+          <t>final energy demand per capita | Industry</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3924,14 +3920,14 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>GJ/cap/year</t>
+          <t>GJ/person/year</t>
         </is>
       </c>
       <c r="H71" t="n">
-        <v>15.22</v>
+        <v>13.1</v>
       </c>
       <c r="I71" t="n">
-        <v>24.2</v>
+        <v>13.09</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -3945,17 +3941,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Climact (2018)</t>
+          <t>Climact (2024)</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>EU28</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>demand</t>
+          <t>Net Zero 2040</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3965,7 +3961,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>FED industry</t>
+          <t>final energy demand industry</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3979,10 +3975,10 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>8.81</v>
+        <v>14.78</v>
       </c>
       <c r="I72" t="n">
-        <v>22.75</v>
+        <v>24.2</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -3996,17 +3992,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>EU28+CH</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Life / Lever 4</t>
+          <t>EU path</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -4016,7 +4012,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>final energy demand industry</t>
+          <t>per capita Total FEC of industry (excl. consumption of the energy sector)</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -4030,14 +4026,14 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>12.89</v>
+        <v>15.22</v>
       </c>
       <c r="I73" t="n">
-        <v>20.72</v>
+        <v>24.2</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K73" t="b">
@@ -4047,23 +4043,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Grubler et al. (2018)</t>
+          <t>Climact (2018)</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>EU28</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
+          <t>demand</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>final energy demand per capita | Industry</t>
+          <t>FED industry</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -4077,40 +4077,44 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>11.28</v>
+        <v>8.81</v>
       </c>
       <c r="I74" t="n">
-        <v>20.97</v>
+        <v>22.75</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>EU28+CH</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>NZE</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr"/>
+          <t>Life / Lever 4</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Final energy demand | Industry</t>
+          <t>final energy demand industry</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -4124,49 +4128,45 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>15.99</v>
+        <v>12.89</v>
       </c>
       <c r="I75" t="n">
-        <v>20.97</v>
+        <v>20.72</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="K75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Eerma et al. (2022)</t>
+          <t>Grubler et al. (2018)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>High Ambition</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Energy</t>
-        </is>
-      </c>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Final energy demand per capita</t>
+          <t>final energy demand per capita | Industry</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>final energy demand per capita and year</t>
+          <t>final energy demand per capita and year | industry</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -4175,49 +4175,45 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>49</v>
+        <v>11.28</v>
       </c>
       <c r="I76" t="n">
-        <v>102.96</v>
+        <v>20.97</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="K76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>UBA (2021)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>GreenSupreme</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Energy</t>
-        </is>
-      </c>
+          <t>NZE</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Final energy demand per capita excluding feedstock</t>
+          <t>Final energy demand | Industry</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>final energy demand per capita and year</t>
+          <t>final energy demand per capita and year | industry</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -4226,34 +4222,34 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>54.07</v>
+        <v>15.99</v>
       </c>
       <c r="I77" t="n">
-        <v>102.96</v>
+        <v>20.97</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="K77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ADEME (2022)</t>
+          <t>Eerma et al. (2022)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>S1: Low production</t>
+          <t>High Ambition</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -4263,7 +4259,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Final energy demand per capita and year</t>
+          <t>Final energy demand per capita</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -4277,10 +4273,10 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>41.32</v>
+        <v>49</v>
       </c>
       <c r="I78" t="n">
-        <v>87.12</v>
+        <v>102.96</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -4294,17 +4290,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>négaWatt (2022)</t>
+          <t>UBA (2021)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>GreenSupreme</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -4314,7 +4310,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>final energy consumption</t>
+          <t>Final energy demand per capita excluding feedstock</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -4328,10 +4324,10 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>48.15</v>
+        <v>54.07</v>
       </c>
       <c r="I79" t="n">
-        <v>87.12</v>
+        <v>102.96</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -4345,17 +4341,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Gaur et al. (2022)</t>
+          <t>Ragwitz et al. (2023)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ILED</t>
+          <t>Nachfrage+Tech</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -4365,7 +4361,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Final energy demand per capita</t>
+          <t>Final Energy Demand</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -4379,10 +4375,10 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>59</v>
+        <v>60.08</v>
       </c>
       <c r="I80" t="n">
-        <v>90</v>
+        <v>102.96</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -4396,17 +4392,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Barrett et al. (2022)</t>
+          <t>ADEME (2022)</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Transform</t>
+          <t>S1: Low production</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -4416,7 +4412,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>final energy demand per capita</t>
+          <t>Final energy demand per capita and year</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -4430,10 +4426,10 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>39.6</v>
+        <v>41.32</v>
       </c>
       <c r="I81" t="n">
-        <v>75.95999999999999</v>
+        <v>87.12</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -4447,17 +4443,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>négaWatt (2022)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>EU path</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -4467,7 +4463,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>final energy per capita excluding ambient heat, non-energy consumption, the energy sector (except blast furnaces) and maritime bunkers from the total</t>
+          <t>final energy consumption</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -4481,10 +4477,10 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>44.28</v>
+        <v>48.15</v>
       </c>
       <c r="I82" t="n">
-        <v>88.2</v>
+        <v>87.12</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -4498,17 +4494,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Climact (2024)</t>
+          <t>Gaur et al. (2022)</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Net Zero 2040</t>
+          <t>ILED</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -4518,7 +4514,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>final energy demand</t>
+          <t>Final energy demand per capita</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -4532,10 +4528,10 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>65.16</v>
+        <v>59</v>
       </c>
       <c r="I83" t="n">
-        <v>88.2</v>
+        <v>90</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -4549,17 +4545,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Climact (2018)</t>
+          <t>Barrett et al. (2022)</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>EU28</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>demand</t>
+          <t>Transform</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -4569,7 +4565,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Energy demand/cap</t>
+          <t>final energy demand per capita</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -4583,10 +4579,10 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>38.83</v>
+        <v>39.6</v>
       </c>
       <c r="I84" t="n">
-        <v>86.61</v>
+        <v>75.95999999999999</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -4600,17 +4596,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>EU28+CH</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Life / Lever 4</t>
+          <t>EU path</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -4620,7 +4616,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>final energy demand</t>
+          <t>final energy per capita excluding ambient heat, non-energy consumption, the energy sector (except blast furnaces) and maritime bunkers from the total</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -4634,14 +4630,14 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>36.78</v>
+        <v>44.28</v>
       </c>
       <c r="I85" t="n">
-        <v>74.36</v>
+        <v>88.2</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K85" t="b">
@@ -4651,17 +4647,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>van Sluisveld et al. (2020)</t>
+          <t>Climact (2024)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Europe+UA</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>RegChange</t>
+          <t>Net Zero 2040</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -4671,7 +4667,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t xml:space="preserve">final energy demand </t>
+          <t>final energy demand</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -4685,14 +4681,14 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>56.31</v>
+        <v>65.16</v>
       </c>
       <c r="I86" t="n">
-        <v>94.14</v>
+        <v>88.2</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>van Sluisveld et al. (2020)</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K86" t="b">
@@ -4702,23 +4698,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Kuhnhenn et al. (2020)</t>
+          <t>Climact (2018)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>GN</t>
+          <t>EU28</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>STS</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr"/>
+          <t>demand</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Final energy demand per capita</t>
+          <t>Energy demand/cap</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -4732,37 +4732,41 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>26.67</v>
+        <v>38.83</v>
       </c>
       <c r="I87" t="n">
-        <v>103.05</v>
+        <v>86.61</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Kuhnhenn et al. (2020)</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Millward-Hopkins et al. (2020)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>WD-DLS</t>
+          <t>EU28+CH</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>decent living standard</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr"/>
+          <t>Life / Lever 4</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
       <c r="E88" t="inlineStr">
         <is>
           <t>final energy demand</t>
@@ -4779,34 +4783,44 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>15.3</v>
-      </c>
-      <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr"/>
+        <v>36.78</v>
+      </c>
+      <c r="I88" t="n">
+        <v>74.36</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Costa et al. (2021) / EUCalc</t>
+        </is>
+      </c>
       <c r="K88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Grubler et al. (2018)</t>
+          <t>van Sluisveld et al. (2020)</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>Europe+UA</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr"/>
+          <t>RegChange</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>final energy demand per capita</t>
+          <t xml:space="preserve">final energy demand </t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -4820,34 +4834,34 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>26.68</v>
+        <v>56.31</v>
       </c>
       <c r="I89" t="n">
-        <v>52.59</v>
+        <v>94.14</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Grubler et al. (2018)</t>
+          <t>van Sluisveld et al. (2020)</t>
         </is>
       </c>
       <c r="K89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Kuhnhenn et al. (2020)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>GN</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>NZE</t>
+          <t>STS</t>
         </is>
       </c>
       <c r="D90" t="inlineStr"/>
@@ -4867,14 +4881,14 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>38.9</v>
+        <v>26.67</v>
       </c>
       <c r="I90" t="n">
-        <v>56.31</v>
+        <v>103.05</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>IEA WEO (2022)</t>
+          <t>Kuhnhenn et al. (2020)</t>
         </is>
       </c>
       <c r="K90" t="b">
@@ -4884,170 +4898,152 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>UBA (2021)</t>
+          <t>Millward-Hopkins et al. (2020)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>WD-DLS</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>GreenSupreme</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
+          <t>decent living standard</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
-          <t>meat consumption per capita and year</t>
+          <t>final energy demand</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>meat consumption per capita and day</t>
+          <t>final energy demand per capita and year</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>kcal meat/cap/day</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="H91" t="n">
-        <v>64.59</v>
-      </c>
-      <c r="I91" t="n">
-        <v>325</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t xml:space="preserve">FAOSTAT - Food and Agriculture Organization of the United Nations </t>
-        </is>
-      </c>
+        <v>15.3</v>
+      </c>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
       <c r="K91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ADEME (2022)</t>
+          <t>Grubler et al. (2018)</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>S1: Low production</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>meat consumption per capita and day</t>
+          <t>final energy demand per capita</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>meat consumption per capita and day</t>
+          <t>final energy demand per capita and year</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>kcal meat/cap/day</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="H92" t="n">
-        <v>61.01</v>
+        <v>26.68</v>
       </c>
       <c r="I92" t="n">
-        <v>387</v>
+        <v>52.59</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t xml:space="preserve">FAOSTAT - Food and Agriculture Organization of the United Nations </t>
+          <t>Grubler et al. (2018)</t>
         </is>
       </c>
       <c r="K92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>négaWatt (2022)</t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2050</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
+          <t>NZE</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
-          <t>meat consumption per capita and day</t>
+          <t>Final energy demand per capita</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>meat consumption per capita and day</t>
+          <t>final energy demand per capita and year</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>kcal/cap/day</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="H93" t="n">
-        <v>155.01</v>
+        <v>38.9</v>
       </c>
       <c r="I93" t="n">
-        <v>387</v>
+        <v>56.31</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t xml:space="preserve">FAOSTAT - Food and Agriculture Organization of the United Nations </t>
+          <t>IEA WEO (2022)</t>
         </is>
       </c>
       <c r="K93" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>van de Ven et al. (2018)</t>
+          <t>UBA (2021)</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Enthusiastic profile</t>
+          <t>GreenSupreme</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -5057,7 +5053,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Meat consumption</t>
+          <t>meat consumption per capita and year</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -5067,18 +5063,18 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>kcal/cap/day</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="H94" t="n">
-        <v>0</v>
+        <v>64.59</v>
       </c>
       <c r="I94" t="n">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t xml:space="preserve">FAOSTAT - Food and Agriculture Organization of the United Nations </t>
         </is>
       </c>
       <c r="K94" t="b">
@@ -5088,17 +5084,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>ADEME (2022)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>EU path</t>
+          <t>S1: Low production</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -5108,7 +5104,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>average daily meat consumption Europe</t>
+          <t>meat consumption per capita and day</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -5122,14 +5118,14 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>211.34</v>
+        <v>61.01</v>
       </c>
       <c r="I95" t="n">
-        <v>347</v>
+        <v>387</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t xml:space="preserve">FAOSTAT - Food and Agriculture Organization of the United Nations </t>
         </is>
       </c>
       <c r="K95" t="b">
@@ -5139,17 +5135,17 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Climact (2024)</t>
+          <t>négaWatt (2022)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Net Zero 2040</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -5159,7 +5155,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>average daily meat consumption Europe</t>
+          <t>meat consumption per capita and day</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -5169,18 +5165,18 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>kcal meat/cap/day</t>
+          <t>kcal/cap/day</t>
         </is>
       </c>
       <c r="H96" t="n">
-        <v>260.25</v>
+        <v>155.01</v>
       </c>
       <c r="I96" t="n">
-        <v>347</v>
+        <v>387</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t xml:space="preserve">FAOSTAT - Food and Agriculture Organization of the United Nations </t>
         </is>
       </c>
       <c r="K96" t="b">
@@ -5190,17 +5186,17 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>van de Ven et al. (2018)</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>EU28+CH</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Life / Lever 4</t>
+          <t>Enthusiastic profile</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -5210,7 +5206,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>meat consumption</t>
+          <t>Meat consumption</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -5220,18 +5216,18 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>kcal meat/cap/day</t>
+          <t>kcal/cap/day</t>
         </is>
       </c>
       <c r="H97" t="n">
-        <v>84.09</v>
+        <v>0</v>
       </c>
       <c r="I97" t="n">
-        <v>322.42</v>
+        <v>347</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Costa et al. (2021) / EUCalc</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K97" t="b">
@@ -5241,23 +5237,27 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Kuhnhenn et al. (2020)</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>GN</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>STS</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr"/>
+          <t>EU path</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Meat consumption</t>
+          <t>average daily meat consumption Europe</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -5267,44 +5267,48 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>kcal/person/day</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="H98" t="n">
-        <v>135</v>
+        <v>211.34</v>
       </c>
       <c r="I98" t="n">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>Kuhnhenn et al. (2020)</t>
+          <t>négaWatt et al. (2023)</t>
         </is>
       </c>
       <c r="K98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Millward-Hopkins et al. (2020)</t>
+          <t>Climact (2024)</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>WD-DLS</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>decent living standard</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr"/>
+          <t>Net Zero 2040</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Meat consumption</t>
+          <t>average daily meat consumption Europe</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -5314,32 +5318,38 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>kcal/cap/day</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="H99" t="n">
-        <v>62.25</v>
-      </c>
-      <c r="I99" t="inlineStr"/>
-      <c r="J99" t="inlineStr"/>
+        <v>260.25</v>
+      </c>
+      <c r="I99" t="n">
+        <v>347</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>négaWatt et al. (2023)</t>
+        </is>
+      </c>
       <c r="K99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>UBA (2021)</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EU28+CH</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>GreenSupreme</t>
+          <t>Life / Lever 4</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -5349,28 +5359,28 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Food waste per capita and year</t>
+          <t>meat consumption</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>food waste per capita and year</t>
+          <t>meat consumption per capita and day</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>kg/cap/year</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="H100" t="n">
-        <v>65.5</v>
+        <v>84.09</v>
       </c>
       <c r="I100" t="n">
-        <v>131</v>
+        <v>322.42</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>BMEL - German federal ministry of agriculture and food</t>
+          <t>Costa et al. (2021) / EUCalc</t>
         </is>
       </c>
       <c r="K100" t="b">
@@ -5380,119 +5390,105 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>négaWatt (2022)</t>
+          <t>Kuhnhenn et al. (2020)</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>GN</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2050</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
+          <t>STS</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr">
         <is>
-          <t>food waste per person and year</t>
+          <t>Meat consumption</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>food waste per capita and year</t>
+          <t>meat consumption per capita and day</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>kg/cap/year</t>
+          <t>kcal/person/day</t>
         </is>
       </c>
       <c r="H101" t="n">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="I101" t="n">
-        <v>110</v>
+        <v>344</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>négaWatt (2022)</t>
+          <t>Kuhnhenn et al. (2020)</t>
         </is>
       </c>
       <c r="K101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Climact (2024)</t>
+          <t>Millward-Hopkins et al. (2020)</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>WD-DLS</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Net Zero 2040</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
+          <t>decent living standard</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr">
         <is>
-          <t>food waste per person</t>
+          <t>Meat consumption</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>food waste per capita and year</t>
+          <t>meat consumption per capita and day</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>kg/cap/year</t>
+          <t>kcal/cap/day</t>
         </is>
       </c>
       <c r="H102" t="n">
-        <v>58.95</v>
-      </c>
-      <c r="I102" t="n">
-        <v>131</v>
-      </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>négaWatt et al. (2023)</t>
-        </is>
-      </c>
+        <v>62.25</v>
+      </c>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
       <c r="K102" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>UBA (2021)</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>EU path</t>
+          <t>GreenSupreme</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -5502,7 +5498,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>food waste per capita and year</t>
+          <t>Food waste per capita and year</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -5523,7 +5519,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>négaWatt et al. (2023)</t>
+          <t>BMEL - German federal ministry of agriculture and food</t>
         </is>
       </c>
       <c r="K103" t="b">
@@ -5533,47 +5529,200 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
+          <t>négaWatt (2022)</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>FR</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>food waste per person and year</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>food waste per capita and year</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>kg/cap/year</t>
+        </is>
+      </c>
+      <c r="H104" t="n">
+        <v>46</v>
+      </c>
+      <c r="I104" t="n">
+        <v>110</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>négaWatt (2022)</t>
+        </is>
+      </c>
+      <c r="K104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Climact (2024)</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Net Zero 2040</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>food waste per person</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>food waste per capita and year</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>kg/cap/year</t>
+        </is>
+      </c>
+      <c r="H105" t="n">
+        <v>58.95</v>
+      </c>
+      <c r="I105" t="n">
+        <v>131</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>négaWatt et al. (2023)</t>
+        </is>
+      </c>
+      <c r="K105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>négaWatt et al. (2023)</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>EU path</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>food waste per capita and year</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>food waste per capita and year</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>kg/cap/year</t>
+        </is>
+      </c>
+      <c r="H106" t="n">
+        <v>65.5</v>
+      </c>
+      <c r="I106" t="n">
+        <v>131</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>négaWatt et al. (2023)</t>
+        </is>
+      </c>
+      <c r="K106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
           <t>IEA WEO (2022)</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
+      <c r="B107" t="inlineStr">
         <is>
           <t>WD</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="C107" t="inlineStr">
         <is>
           <t>NZE</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr">
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
         <is>
           <t>food waste global per capita</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
+      <c r="F107" t="inlineStr">
         <is>
           <t>food waste per capita and year</t>
         </is>
       </c>
-      <c r="G104" t="inlineStr">
+      <c r="G107" t="inlineStr">
         <is>
           <t>kg/cap/year</t>
         </is>
       </c>
-      <c r="H104" t="n">
+      <c r="H107" t="n">
         <v>66.39</v>
       </c>
-      <c r="I104" t="n">
+      <c r="I107" t="n">
         <v>120.5</v>
       </c>
-      <c r="J104" t="inlineStr">
+      <c r="J107" t="inlineStr">
         <is>
           <t>UNEP (2021)</t>
         </is>
       </c>
-      <c r="K104" t="b">
+      <c r="K107" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>